<commit_message>
Set Exis Unit to 1 and MaxlineLoad 100%
</commit_message>
<xml_diff>
--- a/data/Szenario_Default/Power_Parameters.xlsx
+++ b/data/Szenario_Default/Power_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Trafo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF867090-2C74-4F6B-A64C-7FC30BE0150F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24612B-89B5-4505-BB8B-D6D94EE885F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1139,8 +1139,8 @@
   </sheetPr>
   <dimension ref="B1:H85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1560,7 +1560,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="10">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>70</v>
@@ -1948,21 +1948,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2108,10 +2093,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2133,19 +2143,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Disable SoftLineLoadLimits in Szenarios
</commit_message>
<xml_diff>
--- a/data/Szenario_Default/Power_Parameters.xlsx
+++ b/data/Szenario_Default/Power_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24612B-89B5-4505-BB8B-D6D94EE885F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D324094B-B936-4C5F-A26E-F1A4BB369E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1140,7 +1140,7 @@
   <dimension ref="B1:H85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1541,7 +1541,7 @@
         <v>67</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1948,6 +1948,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2093,35 +2108,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2143,9 +2133,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>